<commit_message>
trying to get parameter excel to be read
</commit_message>
<xml_diff>
--- a/tests/testdata/inputfiles/configuration_1.xlsx
+++ b/tests/testdata/inputfiles/configuration_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\GaussianPlume\tests\testdata\inputfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816F26C7-1BA9-44A8-B564-E18336F1158E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1191C3D5-AC67-4238-8663-8BDF8B9327EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" xr2:uid="{72E806E7-A48D-4CBB-AA7B-38F46B3F2219}"/>
+    <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{72E806E7-A48D-4CBB-AA7B-38F46B3F2219}"/>
   </bookViews>
   <sheets>
     <sheet name="fixed parameters" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>roughness</t>
   </si>
@@ -51,10 +51,28 @@
     <t>stack height</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
     <t>E</t>
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
+    <t>var A</t>
+  </si>
+  <si>
+    <t>var B</t>
+  </si>
+  <si>
+    <t>var C</t>
+  </si>
+  <si>
+    <t>datetime</t>
   </si>
 </sst>
 </file>
@@ -409,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42BB1CA2-2AF7-4AB3-B4AF-69F8B7888253}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,6 +445,35 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
     </row>
@@ -439,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A80A9F-53FD-4A28-890F-D3D8B89F068C}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,6 +497,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -492,7 +542,7 @@
         <v>43314.473611111112</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -500,7 +550,7 @@
         <v>43314.517361111109</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>16</v>

</xml_diff>

<commit_message>
Added function to import parameters from Excel, including documentation and tests
</commit_message>
<xml_diff>
--- a/tests/testdata/inputfiles/configuration_1.xlsx
+++ b/tests/testdata/inputfiles/configuration_1.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\GaussianPlume\tests\testdata\inputfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1191C3D5-AC67-4238-8663-8BDF8B9327EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B312CCE0-0384-4864-8E32-8EA69F22F243}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4440" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{72E806E7-A48D-4CBB-AA7B-38F46B3F2219}"/>
   </bookViews>
   <sheets>
-    <sheet name="fixed parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="static parameters" sheetId="1" r:id="rId1"/>
     <sheet name="dynamic parameters" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>roughness</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -73,6 +70,18 @@
   </si>
   <si>
     <t>datetime</t>
+  </si>
+  <si>
+    <t>operator</t>
+  </si>
+  <si>
+    <t>Robbert</t>
+  </si>
+  <si>
+    <t>device NO</t>
+  </si>
+  <si>
+    <t>TNO N77</t>
   </si>
 </sst>
 </file>
@@ -428,18 +437,18 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1">
         <v>5</v>
@@ -447,7 +456,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -455,15 +464,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>33</v>
@@ -471,7 +480,23 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -487,7 +512,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,22 +523,19 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43314.291666666664</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
       <c r="C2">
         <v>5</v>
       </c>
@@ -523,7 +545,7 @@
         <v>43314.402777777781</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>7</v>
@@ -542,7 +564,7 @@
         <v>43314.473611111112</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -550,7 +572,7 @@
         <v>43314.517361111109</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>16</v>

</xml_diff>